<commit_message>
Correcciones en Class1 y final Class4 y Class5
</commit_message>
<xml_diff>
--- a/Tareas/Metodos de la biseccion.xlsx
+++ b/Tareas/Metodos de la biseccion.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://epnecuador-my.sharepoint.com/personal/brandon_freire_epn_edu_ec/Documents/Universidad/Quinto/Metodos Num/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://epnecuador-my.sharepoint.com/personal/brandon_freire_epn_edu_ec/Documents/Universidad/Quinto/Metodos Num/Tareas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="952" documentId="13_ncr:1_{2B86B505-5F0D-43CB-88B0-28F3778B2D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71813E3F-A19B-40DB-ABB6-D44B8493AADA}"/>
+  <xr:revisionPtr revIDLastSave="953" documentId="13_ncr:1_{2B86B505-5F0D-43CB-88B0-28F3778B2D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3436E8E2-44CB-48F8-A658-0DC4D6ABD76C}"/>
   <bookViews>
-    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13667" firstSheet="2" activeTab="5" xr2:uid="{357D95F5-4EC3-4DD1-96EF-25C2127E8AF7}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="12777" windowHeight="13536" firstSheet="2" activeTab="3" xr2:uid="{357D95F5-4EC3-4DD1-96EF-25C2127E8AF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -394,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -443,9 +443,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7248,8 +7245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE479F73-42E6-4BF1-BFB5-077EE0EC5A29}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -15059,8 +15056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9F9E89A-EC72-4724-971D-5F8D911A244C}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -15414,7 +15411,7 @@
       <c r="H3" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="J3" s="3" t="s">
         <v>38</v>
       </c>
       <c r="K3" s="3" t="s">
@@ -18113,7 +18110,7 @@
         <v>-8.0182095593080316E-2</v>
       </c>
       <c r="H91" s="3">
-        <f>D91-D90</f>
+        <f t="shared" ref="H91:H99" si="43">D91-D90</f>
         <v>4.3902944865615856E-2</v>
       </c>
     </row>
@@ -18122,31 +18119,31 @@
         <v>3</v>
       </c>
       <c r="B92" s="3">
-        <f t="shared" ref="B92:B99" si="43">IF(E91*G91&gt;0,D91,B91)</f>
+        <f t="shared" ref="B92:B99" si="44">IF(E91*G91&gt;0,D91,B91)</f>
         <v>1.207729943555</v>
       </c>
       <c r="C92" s="3">
-        <f t="shared" ref="C92:C99" si="44">IF(E91*G91&lt;0,D91,C91)</f>
+        <f t="shared" ref="C92:C99" si="45">IF(E91*G91&lt;0,D91,C91)</f>
         <v>1.4</v>
       </c>
       <c r="D92" s="3">
-        <f t="shared" ref="D92:D99" si="45">C92-F92*(C92-B92)/(F92-E92)</f>
+        <f t="shared" ref="D92:D99" si="46">C92-F92*(C92-B92)/(F92-E92)</f>
         <v>1.217860576639858</v>
       </c>
       <c r="E92" s="3">
-        <f t="shared" ref="E92:E99" si="46">B92^4 - B92 -1</f>
+        <f t="shared" ref="E92:E99" si="47">B92^4 - B92 -1</f>
         <v>-8.0182095593080316E-2</v>
       </c>
       <c r="F92" s="3">
-        <f t="shared" ref="F92:F99" si="47">C92^4 - C92 -1</f>
+        <f t="shared" ref="F92:F99" si="48">C92^4 - C92 -1</f>
         <v>1.4415999999999989</v>
       </c>
       <c r="G92" s="3">
-        <f t="shared" ref="G92:G99" si="48">D92^4 - D92 -1</f>
+        <f t="shared" ref="G92:G99" si="49">D92^4 - D92 -1</f>
         <v>-1.8024659302188439E-2</v>
       </c>
       <c r="H92" s="3">
-        <f>D92-D91</f>
+        <f t="shared" si="43"/>
         <v>1.0130633084858065E-2</v>
       </c>
     </row>
@@ -18155,31 +18152,31 @@
         <v>4</v>
       </c>
       <c r="B93" s="3">
+        <f t="shared" si="44"/>
+        <v>1.217860576639858</v>
+      </c>
+      <c r="C93" s="3">
+        <f t="shared" si="45"/>
+        <v>1.4</v>
+      </c>
+      <c r="D93" s="3">
+        <f t="shared" si="46"/>
+        <v>1.2201097857297709</v>
+      </c>
+      <c r="E93" s="3">
+        <f t="shared" si="47"/>
+        <v>-1.8024659302188439E-2</v>
+      </c>
+      <c r="F93" s="3">
+        <f t="shared" si="48"/>
+        <v>1.4415999999999989</v>
+      </c>
+      <c r="G93" s="3">
+        <f t="shared" si="49"/>
+        <v>-3.9777012947053159E-3</v>
+      </c>
+      <c r="H93" s="3">
         <f t="shared" si="43"/>
-        <v>1.217860576639858</v>
-      </c>
-      <c r="C93" s="3">
-        <f t="shared" si="44"/>
-        <v>1.4</v>
-      </c>
-      <c r="D93" s="3">
-        <f t="shared" si="45"/>
-        <v>1.2201097857297709</v>
-      </c>
-      <c r="E93" s="3">
-        <f t="shared" si="46"/>
-        <v>-1.8024659302188439E-2</v>
-      </c>
-      <c r="F93" s="3">
-        <f t="shared" si="47"/>
-        <v>1.4415999999999989</v>
-      </c>
-      <c r="G93" s="3">
-        <f t="shared" si="48"/>
-        <v>-3.9777012947053159E-3</v>
-      </c>
-      <c r="H93" s="3">
-        <f>D93-D92</f>
         <v>2.2492090899128847E-3</v>
       </c>
     </row>
@@ -18188,31 +18185,31 @@
         <v>5</v>
       </c>
       <c r="B94" s="3">
+        <f t="shared" si="44"/>
+        <v>1.2201097857297709</v>
+      </c>
+      <c r="C94" s="3">
+        <f t="shared" si="45"/>
+        <v>1.4</v>
+      </c>
+      <c r="D94" s="3">
+        <f t="shared" si="46"/>
+        <v>1.2206047778270941</v>
+      </c>
+      <c r="E94" s="3">
+        <f t="shared" si="47"/>
+        <v>-3.9777012947053159E-3</v>
+      </c>
+      <c r="F94" s="3">
+        <f t="shared" si="48"/>
+        <v>1.4415999999999989</v>
+      </c>
+      <c r="G94" s="3">
+        <f t="shared" si="49"/>
+        <v>-8.7421196705683712E-4</v>
+      </c>
+      <c r="H94" s="3">
         <f t="shared" si="43"/>
-        <v>1.2201097857297709</v>
-      </c>
-      <c r="C94" s="3">
-        <f t="shared" si="44"/>
-        <v>1.4</v>
-      </c>
-      <c r="D94" s="3">
-        <f t="shared" si="45"/>
-        <v>1.2206047778270941</v>
-      </c>
-      <c r="E94" s="3">
-        <f t="shared" si="46"/>
-        <v>-3.9777012947053159E-3</v>
-      </c>
-      <c r="F94" s="3">
-        <f t="shared" si="47"/>
-        <v>1.4415999999999989</v>
-      </c>
-      <c r="G94" s="3">
-        <f t="shared" si="48"/>
-        <v>-8.7421196705683712E-4</v>
-      </c>
-      <c r="H94" s="3">
-        <f>D94-D93</f>
         <v>4.9499209732317695E-4</v>
       </c>
     </row>
@@ -18221,31 +18218,31 @@
         <v>6</v>
       </c>
       <c r="B95" s="3">
+        <f t="shared" si="44"/>
+        <v>1.2206047778270941</v>
+      </c>
+      <c r="C95" s="3">
+        <f t="shared" si="45"/>
+        <v>1.4</v>
+      </c>
+      <c r="D95" s="3">
+        <f t="shared" si="46"/>
+        <v>1.2207135003600553</v>
+      </c>
+      <c r="E95" s="3">
+        <f t="shared" si="47"/>
+        <v>-8.7421196705683712E-4</v>
+      </c>
+      <c r="F95" s="3">
+        <f t="shared" si="48"/>
+        <v>1.4415999999999989</v>
+      </c>
+      <c r="G95" s="3">
+        <f t="shared" si="49"/>
+        <v>-1.9195946729344548E-4</v>
+      </c>
+      <c r="H95" s="3">
         <f t="shared" si="43"/>
-        <v>1.2206047778270941</v>
-      </c>
-      <c r="C95" s="3">
-        <f t="shared" si="44"/>
-        <v>1.4</v>
-      </c>
-      <c r="D95" s="3">
-        <f t="shared" si="45"/>
-        <v>1.2207135003600553</v>
-      </c>
-      <c r="E95" s="3">
-        <f t="shared" si="46"/>
-        <v>-8.7421196705683712E-4</v>
-      </c>
-      <c r="F95" s="3">
-        <f t="shared" si="47"/>
-        <v>1.4415999999999989</v>
-      </c>
-      <c r="G95" s="3">
-        <f t="shared" si="48"/>
-        <v>-1.9195946729344548E-4</v>
-      </c>
-      <c r="H95" s="3">
-        <f>D95-D94</f>
         <v>1.0872253296123624E-4</v>
       </c>
     </row>
@@ -18254,31 +18251,31 @@
         <v>7</v>
       </c>
       <c r="B96" s="3">
+        <f t="shared" si="44"/>
+        <v>1.2207135003600553</v>
+      </c>
+      <c r="C96" s="3">
+        <f t="shared" si="45"/>
+        <v>1.4</v>
+      </c>
+      <c r="D96" s="3">
+        <f t="shared" si="46"/>
+        <v>1.220737370475808</v>
+      </c>
+      <c r="E96" s="3">
+        <f t="shared" si="47"/>
+        <v>-1.9195946729344548E-4</v>
+      </c>
+      <c r="F96" s="3">
+        <f t="shared" si="48"/>
+        <v>1.4415999999999989</v>
+      </c>
+      <c r="G96" s="3">
+        <f t="shared" si="49"/>
+        <v>-4.2142109617060441E-5</v>
+      </c>
+      <c r="H96" s="3">
         <f t="shared" si="43"/>
-        <v>1.2207135003600553</v>
-      </c>
-      <c r="C96" s="3">
-        <f t="shared" si="44"/>
-        <v>1.4</v>
-      </c>
-      <c r="D96" s="3">
-        <f t="shared" si="45"/>
-        <v>1.220737370475808</v>
-      </c>
-      <c r="E96" s="3">
-        <f t="shared" si="46"/>
-        <v>-1.9195946729344548E-4</v>
-      </c>
-      <c r="F96" s="3">
-        <f t="shared" si="47"/>
-        <v>1.4415999999999989</v>
-      </c>
-      <c r="G96" s="3">
-        <f t="shared" si="48"/>
-        <v>-4.2142109617060441E-5</v>
-      </c>
-      <c r="H96" s="3">
-        <f>D96-D95</f>
         <v>2.3870115752666621E-5</v>
       </c>
     </row>
@@ -18287,31 +18284,31 @@
         <v>8</v>
       </c>
       <c r="B97" s="3">
+        <f t="shared" si="44"/>
+        <v>1.220737370475808</v>
+      </c>
+      <c r="C97" s="3">
+        <f t="shared" si="45"/>
+        <v>1.4</v>
+      </c>
+      <c r="D97" s="3">
+        <f t="shared" si="46"/>
+        <v>1.2207426106842918</v>
+      </c>
+      <c r="E97" s="3">
+        <f t="shared" si="47"/>
+        <v>-4.2142109617060441E-5</v>
+      </c>
+      <c r="F97" s="3">
+        <f t="shared" si="48"/>
+        <v>1.4415999999999989</v>
+      </c>
+      <c r="G97" s="3">
+        <f t="shared" si="49"/>
+        <v>-9.2513287917039833E-6</v>
+      </c>
+      <c r="H97" s="3">
         <f t="shared" si="43"/>
-        <v>1.220737370475808</v>
-      </c>
-      <c r="C97" s="3">
-        <f t="shared" si="44"/>
-        <v>1.4</v>
-      </c>
-      <c r="D97" s="3">
-        <f t="shared" si="45"/>
-        <v>1.2207426106842918</v>
-      </c>
-      <c r="E97" s="3">
-        <f t="shared" si="46"/>
-        <v>-4.2142109617060441E-5</v>
-      </c>
-      <c r="F97" s="3">
-        <f t="shared" si="47"/>
-        <v>1.4415999999999989</v>
-      </c>
-      <c r="G97" s="3">
-        <f t="shared" si="48"/>
-        <v>-9.2513287917039833E-6</v>
-      </c>
-      <c r="H97" s="3">
-        <f>D97-D96</f>
         <v>5.2402084838032437E-6</v>
       </c>
     </row>
@@ -18320,31 +18317,31 @@
         <v>9</v>
       </c>
       <c r="B98" s="3">
+        <f t="shared" si="44"/>
+        <v>1.2207426106842918</v>
+      </c>
+      <c r="C98" s="3">
+        <f t="shared" si="45"/>
+        <v>1.4</v>
+      </c>
+      <c r="D98" s="3">
+        <f t="shared" si="46"/>
+        <v>1.2207437610438954</v>
+      </c>
+      <c r="E98" s="3">
+        <f t="shared" si="47"/>
+        <v>-9.2513287917039833E-6</v>
+      </c>
+      <c r="F98" s="3">
+        <f t="shared" si="48"/>
+        <v>1.4415999999999989</v>
+      </c>
+      <c r="G98" s="3">
+        <f t="shared" si="49"/>
+        <v>-2.0308965982263061E-6</v>
+      </c>
+      <c r="H98" s="3">
         <f t="shared" si="43"/>
-        <v>1.2207426106842918</v>
-      </c>
-      <c r="C98" s="3">
-        <f t="shared" si="44"/>
-        <v>1.4</v>
-      </c>
-      <c r="D98" s="3">
-        <f t="shared" si="45"/>
-        <v>1.2207437610438954</v>
-      </c>
-      <c r="E98" s="3">
-        <f t="shared" si="46"/>
-        <v>-9.2513287917039833E-6</v>
-      </c>
-      <c r="F98" s="3">
-        <f t="shared" si="47"/>
-        <v>1.4415999999999989</v>
-      </c>
-      <c r="G98" s="3">
-        <f t="shared" si="48"/>
-        <v>-2.0308965982263061E-6</v>
-      </c>
-      <c r="H98" s="3">
-        <f>D98-D97</f>
         <v>1.1503596035744579E-6</v>
       </c>
     </row>
@@ -18353,31 +18350,31 @@
         <v>10</v>
       </c>
       <c r="B99" s="3">
+        <f t="shared" si="44"/>
+        <v>1.2207437610438954</v>
+      </c>
+      <c r="C99" s="3">
+        <f t="shared" si="45"/>
+        <v>1.4</v>
+      </c>
+      <c r="D99" s="3">
+        <f t="shared" si="46"/>
+        <v>1.2207440135760632</v>
+      </c>
+      <c r="E99" s="3">
+        <f t="shared" si="47"/>
+        <v>-2.0308965982263061E-6</v>
+      </c>
+      <c r="F99" s="3">
+        <f t="shared" si="48"/>
+        <v>1.4415999999999989</v>
+      </c>
+      <c r="G99" s="3">
+        <f t="shared" si="49"/>
+        <v>-4.4583134251041656E-7</v>
+      </c>
+      <c r="H99" s="3">
         <f t="shared" si="43"/>
-        <v>1.2207437610438954</v>
-      </c>
-      <c r="C99" s="3">
-        <f t="shared" si="44"/>
-        <v>1.4</v>
-      </c>
-      <c r="D99" s="3">
-        <f t="shared" si="45"/>
-        <v>1.2207440135760632</v>
-      </c>
-      <c r="E99" s="3">
-        <f t="shared" si="46"/>
-        <v>-2.0308965982263061E-6</v>
-      </c>
-      <c r="F99" s="3">
-        <f t="shared" si="47"/>
-        <v>1.4415999999999989</v>
-      </c>
-      <c r="G99" s="3">
-        <f t="shared" si="48"/>
-        <v>-4.4583134251041656E-7</v>
-      </c>
-      <c r="H99" s="3">
-        <f>D99-D98</f>
         <v>2.5253216784371091E-7</v>
       </c>
     </row>

</xml_diff>